<commit_message>
Updated POM files, Page Objects, test data, and compiled classes
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{298EED56-8574-48B8-8117-10295A8EDAA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/applemacbookpro/Documents/SeleniumGuideMukesh/HybridFrameworkSep2022/testdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15271FCB-56A6-FC44-8E7E-5C69EBD96367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13725" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7000" yWindow="5460" windowWidth="24720" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,6 @@
     <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +39,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>ineuron@ineuron.ai</t>
-  </si>
-  <si>
-    <t>ineuron</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -50,13 +48,19 @@
     <t>pwdforUC</t>
   </si>
   <si>
-    <t>Chandan</t>
-  </si>
-  <si>
-    <t>chandan@test.com</t>
-  </si>
-  <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>SnehaB</t>
+  </si>
+  <si>
+    <t>SnehaB@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -147,9 +151,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +191,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +297,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +439,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,15 +450,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -462,18 +466,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{391F147B-AAA6-4678-8173-86354247A2D4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -483,35 +484,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -528,15 +529,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -544,17 +545,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4F5333F1-53DC-41B1-A508-B498EAC9087C}"/>
+    <hyperlink ref="A2" r:id="rId1" display="chandan@test.com" xr:uid="{4F5333F1-53DC-41B1-A508-B498EAC9087C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -566,7 +567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -578,7 +579,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -590,7 +591,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -602,7 +603,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>